<commit_message>
Adding caching for workspace and team names to IDs and support for 1->n workspace->teams assignment
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/add-team-to-workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{094AEADF-9A23-434F-831F-92A1B4A646FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{094AEADF-9A23-434F-831F-92A1B4A646FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0624C07A-148F-4198-A3B9-32D945CDC7D0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Workspace Name</t>
+    <t>Workspace Name - case sensitive</t>
   </si>
   <si>
-    <t>Team Name (if --use_team_id parameter is passed: Team ID instead)</t>
+    <t>Team Name(s) - comma-delimited and case sensitive (if --use_team_id parameter is passed: Team ID instead)</t>
   </si>
   <si>
-    <t>Status (will be set to done when a value is updated)</t>
+    <t>Status (will be set to 'success' or have an error message)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,11 +395,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>